<commit_message>
Added a new Time Difference cost function. Not as powerful
</commit_message>
<xml_diff>
--- a/TdoaSim/Presentation and Documentation/Table Pasting sheet for TDoA Algorithm.xlsx
+++ b/TdoaSim/Presentation and Documentation/Table Pasting sheet for TDoA Algorithm.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\awian\Desktop\MSD\FeasibilityStudies\TdoaSim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\MSD\FeasibilityStudies\TdoaSim\Presentation and Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A966EC6E-C5AE-4EE9-88C7-3C0526A44447}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E02422-76BB-4BC6-9AE2-D957B5149114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9C80441F-F6AE-4DB9-852C-59754C43E2C3}"/>
+    <workbookView xWindow="4545" yWindow="4095" windowWidth="18900" windowHeight="11055" xr2:uid="{9C80441F-F6AE-4DB9-852C-59754C43E2C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>NaN</t>
   </si>
@@ -296,7 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -410,6 +410,10 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -727,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B51845-1427-495A-BD73-7D4E95FCEF8A}">
   <dimension ref="A1:AA56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:K53"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,22 +1121,22 @@
         <v>0.99691358024691401</v>
       </c>
       <c r="B18" s="3">
-        <v>0.72376543209876498</v>
+        <v>0.58796296296296302</v>
       </c>
       <c r="C18" s="23">
-        <v>4.7671038831319503</v>
+        <v>6.5041224460093501</v>
       </c>
       <c r="D18" s="23">
-        <v>7.3886384856665499</v>
+        <v>28.214845749269699</v>
       </c>
       <c r="E18" s="23">
-        <v>3.9187364944388201</v>
+        <v>3.9240778458147201</v>
       </c>
       <c r="F18" s="23">
-        <v>1.8312892685683</v>
+        <v>2.1766512126122302</v>
       </c>
       <c r="G18" s="2">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="H18">
         <v>60</v>
@@ -1143,22 +1147,22 @@
         <v>0.99537037037037002</v>
       </c>
       <c r="B19" s="3">
-        <v>0.78395061728395099</v>
+        <v>0.62654320987654299</v>
       </c>
       <c r="C19" s="23">
-        <v>3.7662814815966699</v>
+        <v>5.3975741344306396</v>
       </c>
       <c r="D19" s="23">
-        <v>4.8888570983064898</v>
+        <v>35.741776044801703</v>
       </c>
       <c r="E19" s="23">
-        <v>3.2957187729732502</v>
+        <v>3.1007782769840899</v>
       </c>
       <c r="F19" s="23">
-        <v>1.6489958987211799</v>
+        <v>1.2860353659228601</v>
       </c>
       <c r="G19" s="2">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="H19">
         <v>65</v>
@@ -1169,25 +1173,25 @@
         <v>0.842592592592593</v>
       </c>
       <c r="B20" s="3">
-        <v>6.17283950617284E-3</v>
+        <v>0</v>
       </c>
       <c r="C20" s="23">
-        <v>140.23229899214101</v>
+        <v>183.186111054778</v>
       </c>
       <c r="D20" s="23">
-        <v>96.5967390467179</v>
+        <v>92.223100532066297</v>
       </c>
       <c r="E20" s="23">
-        <v>18.732482482163</v>
+        <v>14.6436579027897</v>
       </c>
       <c r="F20" s="23">
-        <v>11.8924443740201</v>
-      </c>
-      <c r="G20" s="2">
-        <v>90</v>
+        <v>6.2363243441009297</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="H20">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -1195,25 +1199,25 @@
         <v>0.99691358024691401</v>
       </c>
       <c r="B21" s="3">
-        <v>0.69598765432098797</v>
+        <v>0.50462962962962998</v>
       </c>
       <c r="C21" s="23">
-        <v>5.6257518742842203</v>
+        <v>9.6073890320557496</v>
       </c>
       <c r="D21" s="23">
-        <v>7.7493487546476496</v>
+        <v>71.090035901500997</v>
       </c>
       <c r="E21" s="23">
-        <v>4.2957494487215797</v>
+        <v>4.3709213736600798</v>
       </c>
       <c r="F21" s="23">
-        <v>1.81313465856018</v>
+        <v>1.82803638148556</v>
       </c>
       <c r="G21" s="2">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H21">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -1221,19 +1225,19 @@
         <v>0.99228395061728403</v>
       </c>
       <c r="B22" s="3">
-        <v>0.50925925925925897</v>
+        <v>0.296296296296296</v>
       </c>
       <c r="C22" s="23">
-        <v>9.2382514597639496</v>
+        <v>30.140142176298699</v>
       </c>
       <c r="D22" s="23">
-        <v>16.767183749549101</v>
+        <v>113.34225657166201</v>
       </c>
       <c r="E22" s="23">
-        <v>6.4116686665628002</v>
+        <v>6.64992657391634</v>
       </c>
       <c r="F22" s="23">
-        <v>2.1090802280016301</v>
+        <v>3.0793490493221198</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>0</v>
@@ -1247,25 +1251,25 @@
         <v>0.99691358024691401</v>
       </c>
       <c r="B23" s="3">
-        <v>0.81481481481481499</v>
+        <v>0.67592592592592604</v>
       </c>
       <c r="C23" s="23">
-        <v>3.5189800132604701</v>
+        <v>4.2749364100667302</v>
       </c>
       <c r="D23" s="23">
-        <v>3.8136691510956102</v>
+        <v>18.156706614373402</v>
       </c>
       <c r="E23" s="23">
-        <v>2.8499983421883202</v>
+        <v>2.8269370789892898</v>
       </c>
       <c r="F23" s="23">
-        <v>1.5828147353200701</v>
+        <v>1.31865104338513</v>
       </c>
       <c r="G23" s="2">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H23">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -1273,50 +1277,50 @@
         <v>0.99228395061728403</v>
       </c>
       <c r="B24" s="3">
-        <v>0.56018518518518501</v>
+        <v>0.31018518518518501</v>
       </c>
       <c r="C24" s="23">
-        <v>8.5484976442793297</v>
+        <v>30.785045539260899</v>
       </c>
       <c r="D24" s="23">
-        <v>12.826225709224101</v>
+        <v>121.68714370284199</v>
       </c>
       <c r="E24" s="23">
-        <v>5.8030763884773204</v>
+        <v>6.0031108031544198</v>
       </c>
       <c r="F24" s="23">
-        <v>1.7579508362319101</v>
-      </c>
-      <c r="G24" s="2">
-        <v>30</v>
+        <v>3.1910591821854202</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="H24">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="A25" s="41">
         <v>0.99845679012345701</v>
       </c>
-      <c r="B25" s="3">
-        <v>0.82253086419753096</v>
-      </c>
-      <c r="C25" s="23">
-        <v>3.2274161884264401</v>
-      </c>
-      <c r="D25" s="23">
-        <v>3.8777858727358701</v>
-      </c>
-      <c r="E25" s="23">
-        <v>2.76065726625606</v>
-      </c>
-      <c r="F25" s="23">
-        <v>1.6268928954965201</v>
-      </c>
-      <c r="G25" s="2">
-        <v>5</v>
-      </c>
-      <c r="H25">
+      <c r="B25" s="41">
+        <v>0.68364197530864201</v>
+      </c>
+      <c r="C25" s="42">
+        <v>3.78048484491296</v>
+      </c>
+      <c r="D25" s="42">
+        <v>15.7749639368175</v>
+      </c>
+      <c r="E25" s="42">
+        <v>2.7121008342665802</v>
+      </c>
+      <c r="F25" s="42">
+        <v>1.3893084645587701</v>
+      </c>
+      <c r="G25" s="43">
+        <v>20</v>
+      </c>
+      <c r="H25" s="44">
         <v>70</v>
       </c>
     </row>
@@ -1325,22 +1329,22 @@
         <v>0.99691358024691401</v>
       </c>
       <c r="B26" s="3">
-        <v>0.80555555555555602</v>
+        <v>0.66358024691357997</v>
       </c>
       <c r="C26" s="23">
-        <v>3.6042473989701298</v>
+        <v>4.6177686190237104</v>
       </c>
       <c r="D26" s="23">
-        <v>4.2251748337440098</v>
+        <v>14.763947564591399</v>
       </c>
       <c r="E26" s="23">
-        <v>3.0511811971656901</v>
+        <v>2.9205206881378398</v>
       </c>
       <c r="F26" s="23">
-        <v>1.55722525088334</v>
+        <v>1.3392072681690901</v>
       </c>
       <c r="G26" s="2">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H26">
         <v>65</v>
@@ -1351,25 +1355,49 @@
         <v>0.99537037037037002</v>
       </c>
       <c r="B27" s="3">
-        <v>0.72530864197530898</v>
+        <v>0.60030864197530898</v>
       </c>
       <c r="C27" s="23">
-        <v>4.9603323128851198</v>
+        <v>6.5492757791657796</v>
       </c>
       <c r="D27" s="23">
-        <v>6.8773124311142899</v>
+        <v>44.445453165045699</v>
       </c>
       <c r="E27" s="23">
-        <v>3.9077700402310001</v>
+        <v>3.89762276430173</v>
       </c>
       <c r="F27" s="23">
-        <v>1.65377294417689</v>
+        <v>1.7636480260990399</v>
       </c>
       <c r="G27" s="2">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H27">
-        <v>60</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="44"/>
+      <c r="B28" s="41">
+        <v>0.657407407407407</v>
+      </c>
+      <c r="C28" s="42">
+        <v>4.0083047628767803</v>
+      </c>
+      <c r="D28" s="42">
+        <v>23.027850607104199</v>
+      </c>
+      <c r="E28" s="42">
+        <v>2.7258275260840401</v>
+      </c>
+      <c r="F28" s="42">
+        <v>1.5271403356623601</v>
+      </c>
+      <c r="G28" s="43">
+        <v>20</v>
+      </c>
+      <c r="H28" s="44">
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="116.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
TDoA estimated uncertainty monte carlo runs
</commit_message>
<xml_diff>
--- a/TdoaSim/Presentation and Documentation/Table Pasting sheet for TDoA Algorithm.xlsx
+++ b/TdoaSim/Presentation and Documentation/Table Pasting sheet for TDoA Algorithm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\MSD\FeasibilityStudies\TdoaSim\Presentation and Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\MSD\TDoA Code\FeasibilityStudies\TdoaSim\Presentation and Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E02422-76BB-4BC6-9AE2-D957B5149114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B94212F-1A16-4C6A-A8E5-721CDB1876B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4545" yWindow="4095" windowWidth="18900" windowHeight="11055" xr2:uid="{9C80441F-F6AE-4DB9-852C-59754C43E2C3}"/>
+    <workbookView xWindow="8085" yWindow="6015" windowWidth="21600" windowHeight="11325" xr2:uid="{9C80441F-F6AE-4DB9-852C-59754C43E2C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -404,16 +404,16 @@
     <xf numFmtId="9" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B51845-1427-495A-BD73-7D4E95FCEF8A}">
   <dimension ref="A1:AA56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1121,25 +1121,25 @@
         <v>0.99691358024691401</v>
       </c>
       <c r="B18" s="3">
-        <v>0.58796296296296302</v>
+        <v>0.46141975308642003</v>
       </c>
       <c r="C18" s="23">
-        <v>6.5041224460093501</v>
+        <v>7.3443976533006996</v>
       </c>
       <c r="D18" s="23">
-        <v>28.214845749269699</v>
+        <v>11.878178357748199</v>
       </c>
       <c r="E18" s="23">
-        <v>3.9240778458147201</v>
+        <v>5.3650685428053499</v>
       </c>
       <c r="F18" s="23">
-        <v>2.1766512126122302</v>
+        <v>10.200537333616699</v>
       </c>
       <c r="G18" s="2">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="H18">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -1147,25 +1147,25 @@
         <v>0.99537037037037002</v>
       </c>
       <c r="B19" s="3">
-        <v>0.62654320987654299</v>
+        <v>0.54783950617284005</v>
       </c>
       <c r="C19" s="23">
-        <v>5.3975741344306396</v>
+        <v>5.7331995097676698</v>
       </c>
       <c r="D19" s="23">
-        <v>35.741776044801703</v>
+        <v>9.0782550527084105</v>
       </c>
       <c r="E19" s="23">
-        <v>3.1007782769840899</v>
+        <v>4.1838353121013698</v>
       </c>
       <c r="F19" s="23">
-        <v>1.2860353659228601</v>
+        <v>7.7017234041168203</v>
       </c>
       <c r="G19" s="2">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="H19">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -1176,16 +1176,16 @@
         <v>0</v>
       </c>
       <c r="C20" s="23">
-        <v>183.186111054778</v>
+        <v>123.29050740973</v>
       </c>
       <c r="D20" s="23">
-        <v>92.223100532066297</v>
+        <v>100.175116397633</v>
       </c>
       <c r="E20" s="23">
-        <v>14.6436579027897</v>
+        <v>42.7775199530858</v>
       </c>
       <c r="F20" s="23">
-        <v>6.2363243441009297</v>
+        <v>7.1602831439958301</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>0</v>
@@ -1199,25 +1199,25 @@
         <v>0.99691358024691401</v>
       </c>
       <c r="B21" s="3">
-        <v>0.50462962962962998</v>
+        <v>0.407407407407407</v>
       </c>
       <c r="C21" s="23">
-        <v>9.6073890320557496</v>
+        <v>8.1225063682991703</v>
       </c>
       <c r="D21" s="23">
-        <v>71.090035901500997</v>
+        <v>12.4190159570666</v>
       </c>
       <c r="E21" s="23">
-        <v>4.3709213736600798</v>
+        <v>6.0103433874487404</v>
       </c>
       <c r="F21" s="23">
-        <v>1.82803638148556</v>
+        <v>13.2229813561994</v>
       </c>
       <c r="G21" s="2">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="H21">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
@@ -1225,19 +1225,19 @@
         <v>0.99228395061728403</v>
       </c>
       <c r="B22" s="3">
-        <v>0.296296296296296</v>
+        <v>0.101851851851852</v>
       </c>
       <c r="C22" s="23">
-        <v>30.140142176298699</v>
+        <v>11.9640504941136</v>
       </c>
       <c r="D22" s="23">
-        <v>113.34225657166201</v>
+        <v>15.6073273723034</v>
       </c>
       <c r="E22" s="23">
-        <v>6.64992657391634</v>
+        <v>9.4402349375060606</v>
       </c>
       <c r="F22" s="23">
-        <v>3.0793490493221198</v>
+        <v>17.670167685787899</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>0</v>
@@ -1251,25 +1251,25 @@
         <v>0.99691358024691401</v>
       </c>
       <c r="B23" s="3">
-        <v>0.67592592592592604</v>
+        <v>0.58950617283950602</v>
       </c>
       <c r="C23" s="23">
-        <v>4.2749364100667302</v>
+        <v>4.9482003274105901</v>
       </c>
       <c r="D23" s="23">
-        <v>18.156706614373402</v>
+        <v>8.2595696927181397</v>
       </c>
       <c r="E23" s="23">
-        <v>2.8269370789892898</v>
+        <v>3.6907206883117598</v>
       </c>
       <c r="F23" s="23">
-        <v>1.31865104338513</v>
+        <v>6.7197458555538798</v>
       </c>
       <c r="G23" s="2">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H23">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -1277,19 +1277,19 @@
         <v>0.99228395061728403</v>
       </c>
       <c r="B24" s="3">
-        <v>0.31018518518518501</v>
+        <v>0.19290123456790101</v>
       </c>
       <c r="C24" s="23">
-        <v>30.785045539260899</v>
+        <v>11.1082214821676</v>
       </c>
       <c r="D24" s="23">
-        <v>121.68714370284199</v>
+        <v>14.3663316054086</v>
       </c>
       <c r="E24" s="23">
-        <v>6.0031108031544198</v>
+        <v>8.3116644001215398</v>
       </c>
       <c r="F24" s="23">
-        <v>3.1910591821854202</v>
+        <v>16.375307989934502</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>0</v>
@@ -1299,29 +1299,29 @@
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="41">
+      <c r="A25" s="39">
         <v>0.99845679012345701</v>
       </c>
-      <c r="B25" s="41">
-        <v>0.68364197530864201</v>
-      </c>
-      <c r="C25" s="42">
-        <v>3.78048484491296</v>
-      </c>
-      <c r="D25" s="42">
-        <v>15.7749639368175</v>
-      </c>
-      <c r="E25" s="42">
-        <v>2.7121008342665802</v>
-      </c>
-      <c r="F25" s="42">
-        <v>1.3893084645587701</v>
-      </c>
-      <c r="G25" s="43">
-        <v>20</v>
-      </c>
-      <c r="H25" s="44">
-        <v>70</v>
+      <c r="B25" s="39">
+        <v>0.60030864197530898</v>
+      </c>
+      <c r="C25" s="40">
+        <v>4.8018626749266398</v>
+      </c>
+      <c r="D25" s="40">
+        <v>8.3406348000448602</v>
+      </c>
+      <c r="E25" s="40">
+        <v>3.5278827670437698</v>
+      </c>
+      <c r="F25" s="40">
+        <v>6.1454064014607699</v>
+      </c>
+      <c r="G25" s="41">
+        <v>35</v>
+      </c>
+      <c r="H25" s="42">
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -1329,25 +1329,25 @@
         <v>0.99691358024691401</v>
       </c>
       <c r="B26" s="3">
-        <v>0.66358024691357997</v>
+        <v>0.57407407407407396</v>
       </c>
       <c r="C26" s="23">
-        <v>4.6177686190237104</v>
+        <v>5.3467429659569303</v>
       </c>
       <c r="D26" s="23">
-        <v>14.763947564591399</v>
+        <v>8.3074194251262803</v>
       </c>
       <c r="E26" s="23">
-        <v>2.9205206881378398</v>
+        <v>3.9839773502531002</v>
       </c>
       <c r="F26" s="23">
-        <v>1.3392072681690901</v>
+        <v>7.0424026094141796</v>
       </c>
       <c r="G26" s="2">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H26">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
@@ -1355,48 +1355,48 @@
         <v>0.99537037037037002</v>
       </c>
       <c r="B27" s="3">
-        <v>0.60030864197530898</v>
+        <v>0.45061728395061701</v>
       </c>
       <c r="C27" s="23">
-        <v>6.5492757791657796</v>
+        <v>7.4607002139715402</v>
       </c>
       <c r="D27" s="23">
-        <v>44.445453165045699</v>
+        <v>11.3092209729366</v>
       </c>
       <c r="E27" s="23">
-        <v>3.89762276430173</v>
+        <v>5.52490595590643</v>
       </c>
       <c r="F27" s="23">
-        <v>1.7636480260990399</v>
+        <v>10.874135367838701</v>
       </c>
       <c r="G27" s="2">
+        <v>50</v>
+      </c>
+      <c r="H27">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="42"/>
+      <c r="B28" s="39">
+        <v>0.657407407407407</v>
+      </c>
+      <c r="C28" s="40">
+        <v>4.0083047628767803</v>
+      </c>
+      <c r="D28" s="40">
+        <v>23.027850607104199</v>
+      </c>
+      <c r="E28" s="40">
+        <v>2.7258275260840401</v>
+      </c>
+      <c r="F28" s="40">
+        <v>1.5271403356623601</v>
+      </c>
+      <c r="G28" s="41">
         <v>20</v>
       </c>
-      <c r="H27">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A28" s="44"/>
-      <c r="B28" s="41">
-        <v>0.657407407407407</v>
-      </c>
-      <c r="C28" s="42">
-        <v>4.0083047628767803</v>
-      </c>
-      <c r="D28" s="42">
-        <v>23.027850607104199</v>
-      </c>
-      <c r="E28" s="42">
-        <v>2.7258275260840401</v>
-      </c>
-      <c r="F28" s="42">
-        <v>1.5271403356623601</v>
-      </c>
-      <c r="G28" s="43">
-        <v>20</v>
-      </c>
-      <c r="H28" s="44">
+      <c r="H28" s="42">
         <v>70</v>
       </c>
     </row>
@@ -1723,54 +1723,54 @@
     </row>
     <row r="41" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:27" ht="116.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="39" t="s">
+      <c r="B42" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="39" t="s">
+      <c r="C42" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="D42" s="39" t="s">
+      <c r="D42" s="43" t="s">
         <v>17</v>
       </c>
       <c r="E42" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="F42" s="39" t="s">
+      <c r="F42" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="G42" s="39" t="s">
+      <c r="G42" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="I42" s="39" t="s">
+      <c r="I42" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="J42" s="39" t="s">
+      <c r="J42" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="K42" s="39" t="s">
+      <c r="K42" s="43" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:27" ht="47.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
-      <c r="C43" s="40"/>
-      <c r="D43" s="40"/>
+      <c r="A43" s="44"/>
+      <c r="B43" s="44"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="44"/>
       <c r="E43" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="F43" s="40"/>
-      <c r="G43" s="40"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
-      <c r="K43" s="40"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44"/>
+      <c r="K43" s="44"/>
     </row>
     <row r="44" spans="1:27" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="34" t="s">

</xml_diff>